<commit_message>
power bi com esboços do dataviz
</commit_message>
<xml_diff>
--- a/Entregas/DD-05/datasets_projeto/de_para.xlsx
+++ b/Entregas/DD-05/datasets_projeto/de_para.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cursos\ada_analista_de_dados\3_curso_vem_ser_tech_dados\hackaton_ada\v_1_projeto\datasets_projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cursos\ada_analista_de_dados\3_curso_vem_ser_tech_dados\hackaton_ada\adahack-2024-dados\Entregas\DD-05\datasets_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65920A09-23F6-4800-B869-7618984B7557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24EEC6C-1BCD-40C7-B62E-8C9E247CBEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -284,9 +284,6 @@
     <t>Sul</t>
   </si>
   <si>
-    <t>Menos de 20 anos</t>
-  </si>
-  <si>
     <t>21 - 30 anos</t>
   </si>
   <si>
@@ -296,7 +293,10 @@
     <t>41 - 50 anos</t>
   </si>
   <si>
-    <t>50 anos ou mais</t>
+    <t>&lt;= 20 anos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 50 </t>
   </si>
 </sst>
 </file>
@@ -1483,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB630073-AD19-45FE-A29F-9F03C022D34D}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,7 +1516,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1524,7 +1524,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1532,7 +1532,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1542,6 +1542,9 @@
       <c r="B6" t="s">
         <v>87</v>
       </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
pówer bi com esboços de visualização
</commit_message>
<xml_diff>
--- a/Entregas/DD-05/datasets_projeto/de_para.xlsx
+++ b/Entregas/DD-05/datasets_projeto/de_para.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cursos\ada_analista_de_dados\3_curso_vem_ser_tech_dados\hackaton_ada\v_1_projeto\datasets_projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cursos\ada_analista_de_dados\3_curso_vem_ser_tech_dados\hackaton_ada\adahack-2024-dados\Entregas\DD-05\datasets_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65920A09-23F6-4800-B869-7618984B7557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24EEC6C-1BCD-40C7-B62E-8C9E247CBEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -284,9 +284,6 @@
     <t>Sul</t>
   </si>
   <si>
-    <t>Menos de 20 anos</t>
-  </si>
-  <si>
     <t>21 - 30 anos</t>
   </si>
   <si>
@@ -296,7 +293,10 @@
     <t>41 - 50 anos</t>
   </si>
   <si>
-    <t>50 anos ou mais</t>
+    <t>&lt;= 20 anos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 50 </t>
   </si>
 </sst>
 </file>
@@ -1483,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB630073-AD19-45FE-A29F-9F03C022D34D}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1516,7 +1516,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1524,7 +1524,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1532,7 +1532,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1542,6 +1542,9 @@
       <c r="B6" t="s">
         <v>87</v>
       </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>